<commit_message>
- add size check to Matrix.create() - add check for missing column in Matrix.dropColumns() - Fix bug in OdsImporter and ExcelImporter when assigning column names
</commit_message>
<xml_diff>
--- a/matrix-spreadsheet/src/test/resources/Book2.xlsx
+++ b/matrix-spreadsheet/src/test/resources/Book2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -59,13 +59,28 @@
     <t xml:space="preserve">gång</t>
   </si>
   <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roof</t>
+  </si>
+  <si>
     <t xml:space="preserve">liten</t>
   </si>
   <si>
+    <t xml:space="preserve">Door</t>
+  </si>
+  <si>
     <t xml:space="preserve">gube</t>
   </si>
   <si>
+    <t xml:space="preserve">Window</t>
+  </si>
+  <si>
     <t xml:space="preserve">som</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Side wall</t>
   </si>
   <si>
     <t xml:space="preserve">bodde</t>
@@ -82,7 +97,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -120,16 +135,33 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Roboto Light"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto Light"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -165,6 +197,13 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -191,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,6 +248,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,7 +300,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEBF1DE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -292,10 +351,10 @@
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="AC6:BH10 B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.88"/>
   </cols>
@@ -444,13 +503,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6:BH10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -535,22 +594,310 @@
       <c r="D6" s="3" t="n">
         <v>22.1</v>
       </c>
+      <c r="AC6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AJ6" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK6" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL6" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM6" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN6" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AO6" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="AP6" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AQ6" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AR6" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AS6" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AT6" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AU6" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AV6" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AW6" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AX6" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="AY6" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="AZ6" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA6" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="BB6" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="BC6" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="BD6" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="BE6" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="BF6" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="BG6" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="BH6" s="6" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="4"/>
+      <c r="AC7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="8" t="n">
+        <v>2043</v>
+      </c>
+      <c r="AE7" s="5" t="n">
+        <v>2068</v>
+      </c>
+      <c r="AF7" s="5" t="n">
+        <v>2093</v>
+      </c>
+      <c r="AG7" s="5" t="n">
+        <v>2118</v>
+      </c>
+      <c r="AH7" s="5" t="n">
+        <v>2143</v>
+      </c>
+      <c r="AI7" s="5" t="n">
+        <v>2168</v>
+      </c>
+      <c r="AJ7" s="5" t="n">
+        <v>2193</v>
+      </c>
+      <c r="AK7" s="5" t="n">
+        <v>2218</v>
+      </c>
+      <c r="AL7" s="5" t="n">
+        <v>2243</v>
+      </c>
+      <c r="AM7" s="5" t="n">
+        <v>2268</v>
+      </c>
+      <c r="AN7" s="5" t="n">
+        <v>2293</v>
+      </c>
+      <c r="AO7" s="5" t="n">
+        <v>2318</v>
+      </c>
+      <c r="AP7" s="5" t="n">
+        <v>2343</v>
+      </c>
+      <c r="AQ7" s="5" t="n">
+        <v>2368</v>
+      </c>
+      <c r="AR7" s="5" t="n">
+        <v>2393</v>
+      </c>
+      <c r="AS7" s="5" t="n">
+        <v>2418</v>
+      </c>
+      <c r="AT7" s="5" t="n">
+        <v>2443</v>
+      </c>
+      <c r="AU7" s="5" t="n">
+        <v>2468</v>
+      </c>
+      <c r="AV7" s="5" t="n">
+        <v>2493</v>
+      </c>
+      <c r="AW7" s="5" t="n">
+        <v>2518</v>
+      </c>
+      <c r="AX7" s="5" t="n">
+        <v>2543</v>
+      </c>
+      <c r="AY7" s="5" t="n">
+        <v>2568</v>
+      </c>
+      <c r="AZ7" s="5" t="n">
+        <v>2593</v>
+      </c>
+      <c r="BA7" s="5" t="n">
+        <v>2618</v>
+      </c>
+      <c r="BB7" s="5" t="n">
+        <v>2643</v>
+      </c>
+      <c r="BC7" s="5" t="n">
+        <v>2668</v>
+      </c>
+      <c r="BD7" s="5" t="n">
+        <v>2693</v>
+      </c>
+      <c r="BE7" s="5" t="n">
+        <v>2718</v>
+      </c>
+      <c r="BF7" s="5" t="n">
+        <v>2743</v>
+      </c>
+      <c r="BG7" s="5" t="n">
+        <v>2768</v>
+      </c>
+      <c r="BH7" s="5" t="n">
+        <v>2793</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>45052</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>20.9</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD8" s="5" t="n">
+        <v>2044</v>
+      </c>
+      <c r="AE8" s="5" t="n">
+        <v>2069</v>
+      </c>
+      <c r="AF8" s="5" t="n">
+        <v>2094</v>
+      </c>
+      <c r="AG8" s="5" t="n">
+        <v>2119</v>
+      </c>
+      <c r="AH8" s="5" t="n">
+        <v>2144</v>
+      </c>
+      <c r="AI8" s="5" t="n">
+        <v>2169</v>
+      </c>
+      <c r="AJ8" s="5" t="n">
+        <v>2194</v>
+      </c>
+      <c r="AK8" s="5" t="n">
+        <v>2219</v>
+      </c>
+      <c r="AL8" s="5" t="n">
+        <v>2244</v>
+      </c>
+      <c r="AM8" s="5" t="n">
+        <v>2269</v>
+      </c>
+      <c r="AN8" s="5" t="n">
+        <v>2294</v>
+      </c>
+      <c r="AO8" s="5" t="n">
+        <v>2319</v>
+      </c>
+      <c r="AP8" s="5" t="n">
+        <v>2344</v>
+      </c>
+      <c r="AQ8" s="5" t="n">
+        <v>2369</v>
+      </c>
+      <c r="AR8" s="5" t="n">
+        <v>2394</v>
+      </c>
+      <c r="AS8" s="5" t="n">
+        <v>2419</v>
+      </c>
+      <c r="AT8" s="5" t="n">
+        <v>2444</v>
+      </c>
+      <c r="AU8" s="5" t="n">
+        <v>2469</v>
+      </c>
+      <c r="AV8" s="5" t="n">
+        <v>2494</v>
+      </c>
+      <c r="AW8" s="5" t="n">
+        <v>2519</v>
+      </c>
+      <c r="AX8" s="5" t="n">
+        <v>2544</v>
+      </c>
+      <c r="AY8" s="5" t="n">
+        <v>2569</v>
+      </c>
+      <c r="AZ8" s="5" t="n">
+        <v>2594</v>
+      </c>
+      <c r="BA8" s="5" t="n">
+        <v>2619</v>
+      </c>
+      <c r="BB8" s="5" t="n">
+        <v>2644</v>
+      </c>
+      <c r="BC8" s="5" t="n">
+        <v>2669</v>
+      </c>
+      <c r="BD8" s="5" t="n">
+        <v>2694</v>
+      </c>
+      <c r="BE8" s="5" t="n">
+        <v>2719</v>
+      </c>
+      <c r="BF8" s="5" t="n">
+        <v>2744</v>
+      </c>
+      <c r="BG8" s="5" t="n">
+        <v>2769</v>
+      </c>
+      <c r="BH8" s="5" t="n">
+        <v>2794</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,13 +905,109 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>45053</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>19.4</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD9" s="5" t="n">
+        <v>2045</v>
+      </c>
+      <c r="AE9" s="5" t="n">
+        <v>2070</v>
+      </c>
+      <c r="AF9" s="5" t="n">
+        <v>2095</v>
+      </c>
+      <c r="AG9" s="5" t="n">
+        <v>2120</v>
+      </c>
+      <c r="AH9" s="5" t="n">
+        <v>2145</v>
+      </c>
+      <c r="AI9" s="5" t="n">
+        <v>2170</v>
+      </c>
+      <c r="AJ9" s="5" t="n">
+        <v>2195</v>
+      </c>
+      <c r="AK9" s="5" t="n">
+        <v>2220</v>
+      </c>
+      <c r="AL9" s="5" t="n">
+        <v>2245</v>
+      </c>
+      <c r="AM9" s="5" t="n">
+        <v>2270</v>
+      </c>
+      <c r="AN9" s="5" t="n">
+        <v>2295</v>
+      </c>
+      <c r="AO9" s="5" t="n">
+        <v>2320</v>
+      </c>
+      <c r="AP9" s="5" t="n">
+        <v>2345</v>
+      </c>
+      <c r="AQ9" s="5" t="n">
+        <v>2370</v>
+      </c>
+      <c r="AR9" s="5" t="n">
+        <v>2395</v>
+      </c>
+      <c r="AS9" s="5" t="n">
+        <v>2420</v>
+      </c>
+      <c r="AT9" s="5" t="n">
+        <v>2445</v>
+      </c>
+      <c r="AU9" s="5" t="n">
+        <v>2470</v>
+      </c>
+      <c r="AV9" s="5" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AW9" s="5" t="n">
+        <v>2520</v>
+      </c>
+      <c r="AX9" s="5" t="n">
+        <v>2545</v>
+      </c>
+      <c r="AY9" s="5" t="n">
+        <v>2570</v>
+      </c>
+      <c r="AZ9" s="5" t="n">
+        <v>2595</v>
+      </c>
+      <c r="BA9" s="5" t="n">
+        <v>2620</v>
+      </c>
+      <c r="BB9" s="5" t="n">
+        <v>2645</v>
+      </c>
+      <c r="BC9" s="5" t="n">
+        <v>2670</v>
+      </c>
+      <c r="BD9" s="5" t="n">
+        <v>2695</v>
+      </c>
+      <c r="BE9" s="5" t="n">
+        <v>2720</v>
+      </c>
+      <c r="BF9" s="5" t="n">
+        <v>2745</v>
+      </c>
+      <c r="BG9" s="5" t="n">
+        <v>2770</v>
+      </c>
+      <c r="BH9" s="5" t="n">
+        <v>2795</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,13 +1015,109 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>45054</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>15.6</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD10" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="AE10" s="5" t="n">
+        <v>2065</v>
+      </c>
+      <c r="AF10" s="5" t="n">
+        <v>2090</v>
+      </c>
+      <c r="AG10" s="5" t="n">
+        <v>2115</v>
+      </c>
+      <c r="AH10" s="5" t="n">
+        <v>2140</v>
+      </c>
+      <c r="AI10" s="5" t="n">
+        <v>2165</v>
+      </c>
+      <c r="AJ10" s="5" t="n">
+        <v>2190</v>
+      </c>
+      <c r="AK10" s="5" t="n">
+        <v>2215</v>
+      </c>
+      <c r="AL10" s="5" t="n">
+        <v>2240</v>
+      </c>
+      <c r="AM10" s="5" t="n">
+        <v>2265</v>
+      </c>
+      <c r="AN10" s="5" t="n">
+        <v>2290</v>
+      </c>
+      <c r="AO10" s="5" t="n">
+        <v>2315</v>
+      </c>
+      <c r="AP10" s="5" t="n">
+        <v>2340</v>
+      </c>
+      <c r="AQ10" s="5" t="n">
+        <v>2365</v>
+      </c>
+      <c r="AR10" s="5" t="n">
+        <v>2390</v>
+      </c>
+      <c r="AS10" s="5" t="n">
+        <v>2415</v>
+      </c>
+      <c r="AT10" s="5" t="n">
+        <v>2440</v>
+      </c>
+      <c r="AU10" s="5" t="n">
+        <v>2465</v>
+      </c>
+      <c r="AV10" s="5" t="n">
+        <v>2490</v>
+      </c>
+      <c r="AW10" s="5" t="n">
+        <v>2515</v>
+      </c>
+      <c r="AX10" s="5" t="n">
+        <v>2540</v>
+      </c>
+      <c r="AY10" s="5" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AZ10" s="5" t="n">
+        <v>2590</v>
+      </c>
+      <c r="BA10" s="5" t="n">
+        <v>2615</v>
+      </c>
+      <c r="BB10" s="5" t="n">
+        <v>2640</v>
+      </c>
+      <c r="BC10" s="5" t="n">
+        <v>2665</v>
+      </c>
+      <c r="BD10" s="5" t="n">
+        <v>2690</v>
+      </c>
+      <c r="BE10" s="5" t="n">
+        <v>2715</v>
+      </c>
+      <c r="BF10" s="5" t="n">
+        <v>2740</v>
+      </c>
+      <c r="BG10" s="5" t="n">
+        <v>2765</v>
+      </c>
+      <c r="BH10" s="5" t="n">
+        <v>2790</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +1125,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>45055</v>
@@ -600,7 +1139,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>45056</v>

</xml_diff>

<commit_message>
Fix for currency and percentage in ODS values by converting them to doubles
</commit_message>
<xml_diff>
--- a/matrix-spreadsheet/src/test/resources/Book2.xlsx
+++ b/matrix-spreadsheet/src/test/resources/Book2.xlsx
@@ -1,18 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pernyf/project/matrix/matrix-spreadsheet/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7496CC57-279D-5243-B2EC-DFF388F1131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -23,85 +39,84 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferred_interest_amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentdiff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">det</t>
-  </si>
-  <si>
-    <t xml:space="preserve">var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gång</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Door</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">som</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Side wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bodde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>OB</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>deferred_interest_amount</t>
+  </si>
+  <si>
+    <t>percentdiff</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>baz</t>
+  </si>
+  <si>
+    <t>det</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>gång</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Roof</t>
+  </si>
+  <si>
+    <t>liten</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>gube</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>som</t>
+  </si>
+  <si>
+    <t>Side wall</t>
+  </si>
+  <si>
+    <t>bodde</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;kr&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -110,22 +125,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -142,14 +142,12 @@
     <font>
       <sz val="10"/>
       <name val="Roboto Light"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto Light"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -168,27 +166,29 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFC1C1C1"/>
       </left>
       <right style="thin">
         <color rgb="FFC1C1C1"/>
       </right>
-      <top style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FFC1C1C1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFC1C1C1"/>
       </left>
@@ -203,97 +203,49 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -352,62 +304,78 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -460,853 +428,844 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.88"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="n">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
         <v>710381</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="10">
         <v>19632.75</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="2">
         <v>20516.34</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <f aca="false">(D4-C4)/D4</f>
-        <v>0.0430676231725542</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="n">
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F11" si="0">(D4-C4)/D4</f>
+        <v>4.3067623172554179E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
         <v>710792</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>103599.04</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>103599.04</v>
-      </c>
-      <c r="E5" s="3" t="n">
+      <c r="C5" s="10">
+        <v>103599.03999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>103599.03999999999</v>
+      </c>
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="4" t="n">
-        <f aca="false">(D5-C5)/D5</f>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="n">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
         <v>712353</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="10">
         <v>66419.31</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2">
         <v>66952.95</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <f aca="false">(D6-C6)/D6</f>
-        <v>0.00797037322477948</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="n">
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.9703732247794826E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
         <v>712472</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="10">
         <v>150241.32</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2">
         <v>150737.22</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="4" t="n">
-        <f aca="false">(D7-C7)/D7</f>
-        <v>0.0032898311379233</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="n">
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2898311379232956E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
         <v>712561</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="10">
         <v>111370.35</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2">
         <v>111874.89</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4" t="n">
-        <f aca="false">(D8-C8)/D8</f>
-        <v>0.00450985918287825</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="n">
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>4.5098591828782453E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
         <v>712835</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="10">
         <v>12278.63</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2">
         <v>12898.92</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="4" t="n">
-        <f aca="false">(D9-C9)/D9</f>
-        <v>0.0480885221398381</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3" t="n">
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8088522139838129E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
         <v>713523</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="10">
         <v>119819.76</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2">
         <v>118653.94</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="2">
         <v>2258.16</v>
       </c>
-      <c r="F10" s="4" t="n">
-        <f aca="false">(D10-C10)/D10</f>
-        <v>-0.0098253795870579</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="n">
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.8253795870578958E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
         <v>752810</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="10">
         <v>18609</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="4" t="e">
-        <f aca="false">(D11-C11)/D11</f>
+      <c r="F11" s="3" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="4">
         <v>45047</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2">
         <v>12.4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="4">
         <v>45048</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3">
         <v>23.4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="4">
         <v>45049</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4">
         <v>12.33</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="4">
         <v>45050</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5">
         <v>21.1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="4">
         <v>45051</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6">
         <v>22.1</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AC6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AD6" s="7" t="n">
+      <c r="AD6" s="5">
         <v>1</v>
       </c>
-      <c r="AE6" s="7" t="n">
+      <c r="AE6" s="5">
         <v>2</v>
       </c>
-      <c r="AF6" s="7" t="n">
+      <c r="AF6" s="5">
         <v>3</v>
       </c>
-      <c r="AG6" s="7" t="n">
+      <c r="AG6" s="5">
         <v>4</v>
       </c>
-      <c r="AH6" s="7" t="n">
+      <c r="AH6" s="5">
         <v>5</v>
       </c>
-      <c r="AI6" s="7" t="n">
+      <c r="AI6" s="5">
         <v>6</v>
       </c>
-      <c r="AJ6" s="7" t="n">
+      <c r="AJ6" s="5">
         <v>7</v>
       </c>
-      <c r="AK6" s="7" t="n">
+      <c r="AK6" s="5">
         <v>8</v>
       </c>
-      <c r="AL6" s="7" t="n">
+      <c r="AL6" s="5">
         <v>9</v>
       </c>
-      <c r="AM6" s="7" t="n">
+      <c r="AM6" s="5">
         <v>10</v>
       </c>
-      <c r="AN6" s="7" t="n">
+      <c r="AN6" s="5">
         <v>11</v>
       </c>
-      <c r="AO6" s="7" t="n">
+      <c r="AO6" s="5">
         <v>12</v>
       </c>
-      <c r="AP6" s="7" t="n">
+      <c r="AP6" s="5">
         <v>13</v>
       </c>
-      <c r="AQ6" s="7" t="n">
+      <c r="AQ6" s="5">
         <v>14</v>
       </c>
-      <c r="AR6" s="7" t="n">
+      <c r="AR6" s="5">
         <v>15</v>
       </c>
-      <c r="AS6" s="7" t="n">
+      <c r="AS6" s="5">
         <v>16</v>
       </c>
-      <c r="AT6" s="7" t="n">
+      <c r="AT6" s="5">
         <v>17</v>
       </c>
-      <c r="AU6" s="7" t="n">
+      <c r="AU6" s="5">
         <v>18</v>
       </c>
-      <c r="AV6" s="7" t="n">
+      <c r="AV6" s="5">
         <v>19</v>
       </c>
-      <c r="AW6" s="7" t="n">
+      <c r="AW6" s="5">
         <v>20</v>
       </c>
-      <c r="AX6" s="7" t="n">
+      <c r="AX6" s="5">
         <v>21</v>
       </c>
-      <c r="AY6" s="7" t="n">
+      <c r="AY6" s="5">
         <v>22</v>
       </c>
-      <c r="AZ6" s="7" t="n">
+      <c r="AZ6" s="5">
         <v>23</v>
       </c>
-      <c r="BA6" s="7" t="n">
+      <c r="BA6" s="5">
         <v>24</v>
       </c>
-      <c r="BB6" s="7" t="n">
+      <c r="BB6" s="5">
         <v>25</v>
       </c>
-      <c r="BC6" s="7" t="n">
+      <c r="BC6" s="5">
         <v>26</v>
       </c>
-      <c r="BD6" s="7" t="n">
+      <c r="BD6" s="5">
         <v>27</v>
       </c>
-      <c r="BE6" s="7" t="n">
+      <c r="BE6" s="5">
         <v>28</v>
       </c>
-      <c r="BF6" s="7" t="n">
+      <c r="BF6" s="5">
         <v>29</v>
       </c>
-      <c r="BG6" s="7" t="n">
+      <c r="BG6" s="5">
         <v>30</v>
       </c>
-      <c r="BH6" s="8" t="n">
+      <c r="BH6" s="6">
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="6"/>
-      <c r="AC7" s="9" t="s">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C7" s="4"/>
+      <c r="AC7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AD7" s="10" t="n">
+      <c r="AD7" s="8">
         <v>2043</v>
       </c>
-      <c r="AE7" s="7" t="n">
+      <c r="AE7" s="5">
         <v>2068</v>
       </c>
-      <c r="AF7" s="7" t="n">
+      <c r="AF7" s="5">
         <v>2093</v>
       </c>
-      <c r="AG7" s="7" t="n">
+      <c r="AG7" s="5">
         <v>2118</v>
       </c>
-      <c r="AH7" s="7" t="n">
+      <c r="AH7" s="5">
         <v>2143</v>
       </c>
-      <c r="AI7" s="7" t="n">
+      <c r="AI7" s="5">
         <v>2168</v>
       </c>
-      <c r="AJ7" s="7" t="n">
+      <c r="AJ7" s="5">
         <v>2193</v>
       </c>
-      <c r="AK7" s="7" t="n">
+      <c r="AK7" s="5">
         <v>2218</v>
       </c>
-      <c r="AL7" s="7" t="n">
+      <c r="AL7" s="5">
         <v>2243</v>
       </c>
-      <c r="AM7" s="7" t="n">
+      <c r="AM7" s="5">
         <v>2268</v>
       </c>
-      <c r="AN7" s="7" t="n">
+      <c r="AN7" s="5">
         <v>2293</v>
       </c>
-      <c r="AO7" s="7" t="n">
+      <c r="AO7" s="5">
         <v>2318</v>
       </c>
-      <c r="AP7" s="7" t="n">
+      <c r="AP7" s="5">
         <v>2343</v>
       </c>
-      <c r="AQ7" s="7" t="n">
+      <c r="AQ7" s="5">
         <v>2368</v>
       </c>
-      <c r="AR7" s="7" t="n">
+      <c r="AR7" s="5">
         <v>2393</v>
       </c>
-      <c r="AS7" s="7" t="n">
+      <c r="AS7" s="5">
         <v>2418</v>
       </c>
-      <c r="AT7" s="7" t="n">
+      <c r="AT7" s="5">
         <v>2443</v>
       </c>
-      <c r="AU7" s="7" t="n">
+      <c r="AU7" s="5">
         <v>2468</v>
       </c>
-      <c r="AV7" s="7" t="n">
+      <c r="AV7" s="5">
         <v>2493</v>
       </c>
-      <c r="AW7" s="7" t="n">
+      <c r="AW7" s="5">
         <v>2518</v>
       </c>
-      <c r="AX7" s="7" t="n">
+      <c r="AX7" s="5">
         <v>2543</v>
       </c>
-      <c r="AY7" s="7" t="n">
+      <c r="AY7" s="5">
         <v>2568</v>
       </c>
-      <c r="AZ7" s="7" t="n">
+      <c r="AZ7" s="5">
         <v>2593</v>
       </c>
-      <c r="BA7" s="7" t="n">
+      <c r="BA7" s="5">
         <v>2618</v>
       </c>
-      <c r="BB7" s="7" t="n">
+      <c r="BB7" s="5">
         <v>2643</v>
       </c>
-      <c r="BC7" s="7" t="n">
+      <c r="BC7" s="5">
         <v>2668</v>
       </c>
-      <c r="BD7" s="7" t="n">
+      <c r="BD7" s="5">
         <v>2693</v>
       </c>
-      <c r="BE7" s="7" t="n">
+      <c r="BE7" s="5">
         <v>2718</v>
       </c>
-      <c r="BF7" s="7" t="n">
+      <c r="BF7" s="5">
         <v>2743</v>
       </c>
-      <c r="BG7" s="7" t="n">
+      <c r="BG7" s="5">
         <v>2768</v>
       </c>
-      <c r="BH7" s="7" t="n">
+      <c r="BH7" s="5">
         <v>2793</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="4">
         <v>45052</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8">
         <v>20.9</v>
       </c>
-      <c r="AC8" s="11" t="s">
+      <c r="AC8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AD8" s="7" t="n">
+      <c r="AD8" s="5">
         <v>2044</v>
       </c>
-      <c r="AE8" s="7" t="n">
+      <c r="AE8" s="5">
         <v>2069</v>
       </c>
-      <c r="AF8" s="7" t="n">
+      <c r="AF8" s="5">
         <v>2094</v>
       </c>
-      <c r="AG8" s="7" t="n">
+      <c r="AG8" s="5">
         <v>2119</v>
       </c>
-      <c r="AH8" s="7" t="n">
+      <c r="AH8" s="5">
         <v>2144</v>
       </c>
-      <c r="AI8" s="7" t="n">
+      <c r="AI8" s="5">
         <v>2169</v>
       </c>
-      <c r="AJ8" s="7" t="n">
+      <c r="AJ8" s="5">
         <v>2194</v>
       </c>
-      <c r="AK8" s="7" t="n">
+      <c r="AK8" s="5">
         <v>2219</v>
       </c>
-      <c r="AL8" s="7" t="n">
+      <c r="AL8" s="5">
         <v>2244</v>
       </c>
-      <c r="AM8" s="7" t="n">
+      <c r="AM8" s="5">
         <v>2269</v>
       </c>
-      <c r="AN8" s="7" t="n">
+      <c r="AN8" s="5">
         <v>2294</v>
       </c>
-      <c r="AO8" s="7" t="n">
+      <c r="AO8" s="5">
         <v>2319</v>
       </c>
-      <c r="AP8" s="7" t="n">
+      <c r="AP8" s="5">
         <v>2344</v>
       </c>
-      <c r="AQ8" s="7" t="n">
+      <c r="AQ8" s="5">
         <v>2369</v>
       </c>
-      <c r="AR8" s="7" t="n">
+      <c r="AR8" s="5">
         <v>2394</v>
       </c>
-      <c r="AS8" s="7" t="n">
+      <c r="AS8" s="5">
         <v>2419</v>
       </c>
-      <c r="AT8" s="7" t="n">
+      <c r="AT8" s="5">
         <v>2444</v>
       </c>
-      <c r="AU8" s="7" t="n">
+      <c r="AU8" s="5">
         <v>2469</v>
       </c>
-      <c r="AV8" s="7" t="n">
+      <c r="AV8" s="5">
         <v>2494</v>
       </c>
-      <c r="AW8" s="7" t="n">
+      <c r="AW8" s="5">
         <v>2519</v>
       </c>
-      <c r="AX8" s="7" t="n">
+      <c r="AX8" s="5">
         <v>2544</v>
       </c>
-      <c r="AY8" s="7" t="n">
+      <c r="AY8" s="5">
         <v>2569</v>
       </c>
-      <c r="AZ8" s="7" t="n">
+      <c r="AZ8" s="5">
         <v>2594</v>
       </c>
-      <c r="BA8" s="7" t="n">
+      <c r="BA8" s="5">
         <v>2619</v>
       </c>
-      <c r="BB8" s="7" t="n">
+      <c r="BB8" s="5">
         <v>2644</v>
       </c>
-      <c r="BC8" s="7" t="n">
+      <c r="BC8" s="5">
         <v>2669</v>
       </c>
-      <c r="BD8" s="7" t="n">
+      <c r="BD8" s="5">
         <v>2694</v>
       </c>
-      <c r="BE8" s="7" t="n">
+      <c r="BE8" s="5">
         <v>2719</v>
       </c>
-      <c r="BF8" s="7" t="n">
+      <c r="BF8" s="5">
         <v>2744</v>
       </c>
-      <c r="BG8" s="7" t="n">
+      <c r="BG8" s="5">
         <v>2769</v>
       </c>
-      <c r="BH8" s="7" t="n">
+      <c r="BH8" s="5">
         <v>2794</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="4">
         <v>45053</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <v>19.4</v>
-      </c>
-      <c r="AC9" s="11" t="s">
+      <c r="D9">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="AC9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="7" t="n">
+      <c r="AD9" s="5">
         <v>2045</v>
       </c>
-      <c r="AE9" s="7" t="n">
+      <c r="AE9" s="5">
         <v>2070</v>
       </c>
-      <c r="AF9" s="7" t="n">
+      <c r="AF9" s="5">
         <v>2095</v>
       </c>
-      <c r="AG9" s="7" t="n">
+      <c r="AG9" s="5">
         <v>2120</v>
       </c>
-      <c r="AH9" s="7" t="n">
+      <c r="AH9" s="5">
         <v>2145</v>
       </c>
-      <c r="AI9" s="7" t="n">
+      <c r="AI9" s="5">
         <v>2170</v>
       </c>
-      <c r="AJ9" s="7" t="n">
+      <c r="AJ9" s="5">
         <v>2195</v>
       </c>
-      <c r="AK9" s="7" t="n">
+      <c r="AK9" s="5">
         <v>2220</v>
       </c>
-      <c r="AL9" s="7" t="n">
+      <c r="AL9" s="5">
         <v>2245</v>
       </c>
-      <c r="AM9" s="7" t="n">
+      <c r="AM9" s="5">
         <v>2270</v>
       </c>
-      <c r="AN9" s="7" t="n">
+      <c r="AN9" s="5">
         <v>2295</v>
       </c>
-      <c r="AO9" s="7" t="n">
+      <c r="AO9" s="5">
         <v>2320</v>
       </c>
-      <c r="AP9" s="7" t="n">
+      <c r="AP9" s="5">
         <v>2345</v>
       </c>
-      <c r="AQ9" s="7" t="n">
+      <c r="AQ9" s="5">
         <v>2370</v>
       </c>
-      <c r="AR9" s="7" t="n">
+      <c r="AR9" s="5">
         <v>2395</v>
       </c>
-      <c r="AS9" s="7" t="n">
+      <c r="AS9" s="5">
         <v>2420</v>
       </c>
-      <c r="AT9" s="7" t="n">
+      <c r="AT9" s="5">
         <v>2445</v>
       </c>
-      <c r="AU9" s="7" t="n">
+      <c r="AU9" s="5">
         <v>2470</v>
       </c>
-      <c r="AV9" s="7" t="n">
+      <c r="AV9" s="5">
         <v>2495</v>
       </c>
-      <c r="AW9" s="7" t="n">
+      <c r="AW9" s="5">
         <v>2520</v>
       </c>
-      <c r="AX9" s="7" t="n">
+      <c r="AX9" s="5">
         <v>2545</v>
       </c>
-      <c r="AY9" s="7" t="n">
+      <c r="AY9" s="5">
         <v>2570</v>
       </c>
-      <c r="AZ9" s="7" t="n">
+      <c r="AZ9" s="5">
         <v>2595</v>
       </c>
-      <c r="BA9" s="7" t="n">
+      <c r="BA9" s="5">
         <v>2620</v>
       </c>
-      <c r="BB9" s="7" t="n">
+      <c r="BB9" s="5">
         <v>2645</v>
       </c>
-      <c r="BC9" s="7" t="n">
+      <c r="BC9" s="5">
         <v>2670</v>
       </c>
-      <c r="BD9" s="7" t="n">
+      <c r="BD9" s="5">
         <v>2695</v>
       </c>
-      <c r="BE9" s="7" t="n">
+      <c r="BE9" s="5">
         <v>2720</v>
       </c>
-      <c r="BF9" s="7" t="n">
+      <c r="BF9" s="5">
         <v>2745</v>
       </c>
-      <c r="BG9" s="7" t="n">
+      <c r="BG9" s="5">
         <v>2770</v>
       </c>
-      <c r="BH9" s="7" t="n">
+      <c r="BH9" s="5">
         <v>2795</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="4">
         <v>45054</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10">
         <v>15.6</v>
       </c>
-      <c r="AC10" s="11" t="s">
+      <c r="AC10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AD10" s="7" t="n">
+      <c r="AD10" s="5">
         <v>2040</v>
       </c>
-      <c r="AE10" s="7" t="n">
+      <c r="AE10" s="5">
         <v>2065</v>
       </c>
-      <c r="AF10" s="7" t="n">
+      <c r="AF10" s="5">
         <v>2090</v>
       </c>
-      <c r="AG10" s="7" t="n">
+      <c r="AG10" s="5">
         <v>2115</v>
       </c>
-      <c r="AH10" s="7" t="n">
+      <c r="AH10" s="5">
         <v>2140</v>
       </c>
-      <c r="AI10" s="7" t="n">
+      <c r="AI10" s="5">
         <v>2165</v>
       </c>
-      <c r="AJ10" s="7" t="n">
+      <c r="AJ10" s="5">
         <v>2190</v>
       </c>
-      <c r="AK10" s="7" t="n">
+      <c r="AK10" s="5">
         <v>2215</v>
       </c>
-      <c r="AL10" s="7" t="n">
+      <c r="AL10" s="5">
         <v>2240</v>
       </c>
-      <c r="AM10" s="7" t="n">
+      <c r="AM10" s="5">
         <v>2265</v>
       </c>
-      <c r="AN10" s="7" t="n">
+      <c r="AN10" s="5">
         <v>2290</v>
       </c>
-      <c r="AO10" s="7" t="n">
+      <c r="AO10" s="5">
         <v>2315</v>
       </c>
-      <c r="AP10" s="7" t="n">
+      <c r="AP10" s="5">
         <v>2340</v>
       </c>
-      <c r="AQ10" s="7" t="n">
+      <c r="AQ10" s="5">
         <v>2365</v>
       </c>
-      <c r="AR10" s="7" t="n">
+      <c r="AR10" s="5">
         <v>2390</v>
       </c>
-      <c r="AS10" s="7" t="n">
+      <c r="AS10" s="5">
         <v>2415</v>
       </c>
-      <c r="AT10" s="7" t="n">
+      <c r="AT10" s="5">
         <v>2440</v>
       </c>
-      <c r="AU10" s="7" t="n">
+      <c r="AU10" s="5">
         <v>2465</v>
       </c>
-      <c r="AV10" s="7" t="n">
+      <c r="AV10" s="5">
         <v>2490</v>
       </c>
-      <c r="AW10" s="7" t="n">
+      <c r="AW10" s="5">
         <v>2515</v>
       </c>
-      <c r="AX10" s="7" t="n">
+      <c r="AX10" s="5">
         <v>2540</v>
       </c>
-      <c r="AY10" s="7" t="n">
+      <c r="AY10" s="5">
         <v>2565</v>
       </c>
-      <c r="AZ10" s="7" t="n">
+      <c r="AZ10" s="5">
         <v>2590</v>
       </c>
-      <c r="BA10" s="7" t="n">
+      <c r="BA10" s="5">
         <v>2615</v>
       </c>
-      <c r="BB10" s="7" t="n">
+      <c r="BB10" s="5">
         <v>2640</v>
       </c>
-      <c r="BC10" s="7" t="n">
+      <c r="BC10" s="5">
         <v>2665</v>
       </c>
-      <c r="BD10" s="7" t="n">
+      <c r="BD10" s="5">
         <v>2690</v>
       </c>
-      <c r="BE10" s="7" t="n">
+      <c r="BE10" s="5">
         <v>2715</v>
       </c>
-      <c r="BF10" s="7" t="n">
+      <c r="BF10" s="5">
         <v>2740</v>
       </c>
-      <c r="BG10" s="7" t="n">
+      <c r="BG10" s="5">
         <v>2765</v>
       </c>
-      <c r="BH10" s="7" t="n">
+      <c r="BH10" s="5">
         <v>2790</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="4">
         <v>45055</v>
       </c>
-      <c r="D11" s="5" t="n">
-        <v>18.9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="D11">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="4">
         <v>45056</v>
       </c>
-      <c r="D12" s="5" t="n">
-        <v>17.4</v>
+      <c r="D12">
+        <v>17.399999999999999</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
make excelimporter return a LocalDate if no time is specified to make the behavior align with OdsImporter
</commit_message>
<xml_diff>
--- a/matrix-spreadsheet/src/test/resources/Book2.xlsx
+++ b/matrix-spreadsheet/src/test/resources/Book2.xlsx
@@ -1,34 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pernyf/project/matrix/matrix-spreadsheet/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7496CC57-279D-5243-B2EC-DFF388F1131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -39,84 +23,86 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>OB</t>
-  </si>
-  <si>
-    <t>IB</t>
-  </si>
-  <si>
-    <t>deferred_interest_amount</t>
-  </si>
-  <si>
-    <t>percentdiff</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>baz</t>
-  </si>
-  <si>
-    <t>det</t>
-  </si>
-  <si>
-    <t>var</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>gång</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Roof</t>
-  </si>
-  <si>
-    <t>liten</t>
-  </si>
-  <si>
-    <t>Door</t>
-  </si>
-  <si>
-    <t>gube</t>
-  </si>
-  <si>
-    <t>Window</t>
-  </si>
-  <si>
-    <t>som</t>
-  </si>
-  <si>
-    <t>Side wall</t>
-  </si>
-  <si>
-    <t>bodde</t>
-  </si>
-  <si>
-    <t>i</t>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferred_interest_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentdiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gång</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">som</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Side wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bodde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;kr&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -125,7 +111,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -142,12 +143,14 @@
     <font>
       <sz val="10"/>
       <name val="Roboto Light"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto Light"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -166,29 +169,27 @@
     </fill>
   </fills>
   <borders count="4">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFC1C1C1"/>
       </left>
       <right style="thin">
         <color rgb="FFC1C1C1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top style="medium"/>
       <bottom style="thin">
         <color rgb="FFC1C1C1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFC1C1C1"/>
       </left>
@@ -203,49 +204,101 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+  <cellXfs count="13">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -304,78 +357,62 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -428,844 +465,854 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.83"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="n">
         <v>710381</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="5" t="n">
         <v>19632.75</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4" t="n">
         <v>20516.34</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" ref="F4:F11" si="0">(D4-C4)/D4</f>
-        <v>4.3067623172554179E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="2">
+      <c r="F4" s="6" t="n">
+        <f aca="false">(D4-C4)/D4</f>
+        <v>0.0430676231725542</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4" t="n">
         <v>710792</v>
       </c>
-      <c r="C5" s="10">
-        <v>103599.03999999999</v>
-      </c>
-      <c r="D5" s="2">
-        <v>103599.03999999999</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="5" t="n">
+        <v>103599.04</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>103599.04</v>
+      </c>
+      <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
+      <c r="F5" s="6" t="n">
+        <f aca="false">(D5-C5)/D5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="n">
         <v>712353</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="5" t="n">
         <v>66419.31</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4" t="n">
         <v>66952.95</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>7.9703732247794826E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
+      <c r="F6" s="6" t="n">
+        <f aca="false">(D6-C6)/D6</f>
+        <v>0.00797037322477948</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="4" t="n">
         <v>712472</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="5" t="n">
         <v>150241.32</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4" t="n">
         <v>150737.22</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>3.2898311379232956E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
+      <c r="F7" s="6" t="n">
+        <f aca="false">(D7-C7)/D7</f>
+        <v>0.0032898311379233</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="n">
         <v>712561</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="5" t="n">
         <v>111370.35</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4" t="n">
         <v>111874.89</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>4.5098591828782453E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
+      <c r="F8" s="6" t="n">
+        <f aca="false">(D8-C8)/D8</f>
+        <v>0.00450985918287825</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="4" t="n">
         <v>712835</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="5" t="n">
         <v>12278.63</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4" t="n">
         <v>12898.92</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>4.8088522139838129E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
+      <c r="F9" s="6" t="n">
+        <f aca="false">(D9-C9)/D9</f>
+        <v>0.0480885221398381</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="4" t="n">
         <v>713523</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="5" t="n">
         <v>119819.76</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4" t="n">
         <v>118653.94</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4" t="n">
         <v>2258.16</v>
       </c>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.8253795870578958E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
+      <c r="F10" s="6" t="n">
+        <f aca="false">(D10-C10)/D10</f>
+        <v>-0.0098253795870579</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="4" t="n">
         <v>752810</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="5" t="n">
         <v>18609</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="e">
-        <f t="shared" si="0"/>
+      <c r="F11" s="6" t="e">
+        <f aca="false">(D11-C11)/D11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="4"/>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="7" t="n">
         <v>45047</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1" t="n">
         <v>12.4</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7" t="n">
         <v>45048</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1" t="n">
         <v>23.4</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="7" t="n">
         <v>45049</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1" t="n">
         <v>12.33</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="7" t="n">
         <v>45050</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1" t="n">
         <v>21.1</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="7" t="n">
         <v>45051</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1" t="n">
         <v>22.1</v>
       </c>
-      <c r="AC6" s="5" t="s">
+      <c r="AC6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AD6" s="5">
+      <c r="AD6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="AE6" s="5">
+      <c r="AE6" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AF6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AG6" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="AH6" s="5">
+      <c r="AH6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="AI6" s="5">
+      <c r="AI6" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AK6" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="AL6" s="5">
+      <c r="AL6" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="AN6" s="5">
+      <c r="AN6" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="AO6" s="5">
+      <c r="AO6" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="AP6" s="5">
+      <c r="AP6" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="AQ6" s="5">
+      <c r="AQ6" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="AR6" s="5">
+      <c r="AR6" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AS6" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AT6" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="AU6" s="5">
+      <c r="AU6" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="AV6" s="5">
+      <c r="AV6" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="AW6" s="5">
+      <c r="AW6" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="AX6" s="5">
+      <c r="AX6" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="AY6" s="5">
+      <c r="AY6" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="AZ6" s="5">
+      <c r="AZ6" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="BA6" s="5">
+      <c r="BA6" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="BB6" s="5">
+      <c r="BB6" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="BC6" s="5">
+      <c r="BC6" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="BD6" s="5">
+      <c r="BD6" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="BE6" s="5">
+      <c r="BE6" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="BF6" s="5">
+      <c r="BF6" s="8" t="n">
         <v>29</v>
       </c>
-      <c r="BG6" s="5">
+      <c r="BG6" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="BH6" s="6">
+      <c r="BH6" s="9" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C7" s="4"/>
-      <c r="AC7" s="7" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="7"/>
+      <c r="AC7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AD7" s="11" t="n">
         <v>2043</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AE7" s="8" t="n">
         <v>2068</v>
       </c>
-      <c r="AF7" s="5">
+      <c r="AF7" s="8" t="n">
         <v>2093</v>
       </c>
-      <c r="AG7" s="5">
+      <c r="AG7" s="8" t="n">
         <v>2118</v>
       </c>
-      <c r="AH7" s="5">
+      <c r="AH7" s="8" t="n">
         <v>2143</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AI7" s="8" t="n">
         <v>2168</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="8" t="n">
         <v>2193</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AK7" s="8" t="n">
         <v>2218</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="8" t="n">
         <v>2243</v>
       </c>
-      <c r="AM7" s="5">
+      <c r="AM7" s="8" t="n">
         <v>2268</v>
       </c>
-      <c r="AN7" s="5">
+      <c r="AN7" s="8" t="n">
         <v>2293</v>
       </c>
-      <c r="AO7" s="5">
+      <c r="AO7" s="8" t="n">
         <v>2318</v>
       </c>
-      <c r="AP7" s="5">
+      <c r="AP7" s="8" t="n">
         <v>2343</v>
       </c>
-      <c r="AQ7" s="5">
+      <c r="AQ7" s="8" t="n">
         <v>2368</v>
       </c>
-      <c r="AR7" s="5">
+      <c r="AR7" s="8" t="n">
         <v>2393</v>
       </c>
-      <c r="AS7" s="5">
+      <c r="AS7" s="8" t="n">
         <v>2418</v>
       </c>
-      <c r="AT7" s="5">
+      <c r="AT7" s="8" t="n">
         <v>2443</v>
       </c>
-      <c r="AU7" s="5">
+      <c r="AU7" s="8" t="n">
         <v>2468</v>
       </c>
-      <c r="AV7" s="5">
+      <c r="AV7" s="8" t="n">
         <v>2493</v>
       </c>
-      <c r="AW7" s="5">
+      <c r="AW7" s="8" t="n">
         <v>2518</v>
       </c>
-      <c r="AX7" s="5">
+      <c r="AX7" s="8" t="n">
         <v>2543</v>
       </c>
-      <c r="AY7" s="5">
+      <c r="AY7" s="8" t="n">
         <v>2568</v>
       </c>
-      <c r="AZ7" s="5">
+      <c r="AZ7" s="8" t="n">
         <v>2593</v>
       </c>
-      <c r="BA7" s="5">
+      <c r="BA7" s="8" t="n">
         <v>2618</v>
       </c>
-      <c r="BB7" s="5">
+      <c r="BB7" s="8" t="n">
         <v>2643</v>
       </c>
-      <c r="BC7" s="5">
+      <c r="BC7" s="8" t="n">
         <v>2668</v>
       </c>
-      <c r="BD7" s="5">
+      <c r="BD7" s="8" t="n">
         <v>2693</v>
       </c>
-      <c r="BE7" s="5">
+      <c r="BE7" s="8" t="n">
         <v>2718</v>
       </c>
-      <c r="BF7" s="5">
+      <c r="BF7" s="8" t="n">
         <v>2743</v>
       </c>
-      <c r="BG7" s="5">
+      <c r="BG7" s="8" t="n">
         <v>2768</v>
       </c>
-      <c r="BH7" s="5">
+      <c r="BH7" s="8" t="n">
         <v>2793</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="7" t="n">
         <v>45052</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1" t="n">
         <v>20.9</v>
       </c>
-      <c r="AC8" s="9" t="s">
+      <c r="AC8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AD8" s="5">
+      <c r="AD8" s="8" t="n">
         <v>2044</v>
       </c>
-      <c r="AE8" s="5">
+      <c r="AE8" s="8" t="n">
         <v>2069</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AF8" s="8" t="n">
         <v>2094</v>
       </c>
-      <c r="AG8" s="5">
+      <c r="AG8" s="8" t="n">
         <v>2119</v>
       </c>
-      <c r="AH8" s="5">
+      <c r="AH8" s="8" t="n">
         <v>2144</v>
       </c>
-      <c r="AI8" s="5">
+      <c r="AI8" s="8" t="n">
         <v>2169</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AJ8" s="8" t="n">
         <v>2194</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AK8" s="8" t="n">
         <v>2219</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AL8" s="8" t="n">
         <v>2244</v>
       </c>
-      <c r="AM8" s="5">
+      <c r="AM8" s="8" t="n">
         <v>2269</v>
       </c>
-      <c r="AN8" s="5">
+      <c r="AN8" s="8" t="n">
         <v>2294</v>
       </c>
-      <c r="AO8" s="5">
+      <c r="AO8" s="8" t="n">
         <v>2319</v>
       </c>
-      <c r="AP8" s="5">
+      <c r="AP8" s="8" t="n">
         <v>2344</v>
       </c>
-      <c r="AQ8" s="5">
+      <c r="AQ8" s="8" t="n">
         <v>2369</v>
       </c>
-      <c r="AR8" s="5">
+      <c r="AR8" s="8" t="n">
         <v>2394</v>
       </c>
-      <c r="AS8" s="5">
+      <c r="AS8" s="8" t="n">
         <v>2419</v>
       </c>
-      <c r="AT8" s="5">
+      <c r="AT8" s="8" t="n">
         <v>2444</v>
       </c>
-      <c r="AU8" s="5">
+      <c r="AU8" s="8" t="n">
         <v>2469</v>
       </c>
-      <c r="AV8" s="5">
+      <c r="AV8" s="8" t="n">
         <v>2494</v>
       </c>
-      <c r="AW8" s="5">
+      <c r="AW8" s="8" t="n">
         <v>2519</v>
       </c>
-      <c r="AX8" s="5">
+      <c r="AX8" s="8" t="n">
         <v>2544</v>
       </c>
-      <c r="AY8" s="5">
+      <c r="AY8" s="8" t="n">
         <v>2569</v>
       </c>
-      <c r="AZ8" s="5">
+      <c r="AZ8" s="8" t="n">
         <v>2594</v>
       </c>
-      <c r="BA8" s="5">
+      <c r="BA8" s="8" t="n">
         <v>2619</v>
       </c>
-      <c r="BB8" s="5">
+      <c r="BB8" s="8" t="n">
         <v>2644</v>
       </c>
-      <c r="BC8" s="5">
+      <c r="BC8" s="8" t="n">
         <v>2669</v>
       </c>
-      <c r="BD8" s="5">
+      <c r="BD8" s="8" t="n">
         <v>2694</v>
       </c>
-      <c r="BE8" s="5">
+      <c r="BE8" s="8" t="n">
         <v>2719</v>
       </c>
-      <c r="BF8" s="5">
+      <c r="BF8" s="8" t="n">
         <v>2744</v>
       </c>
-      <c r="BG8" s="5">
+      <c r="BG8" s="8" t="n">
         <v>2769</v>
       </c>
-      <c r="BH8" s="5">
+      <c r="BH8" s="8" t="n">
         <v>2794</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="7" t="n">
         <v>45053</v>
       </c>
-      <c r="D9">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="AC9" s="9" t="s">
+      <c r="D9" s="1" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="AC9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="5">
+      <c r="AD9" s="8" t="n">
         <v>2045</v>
       </c>
-      <c r="AE9" s="5">
+      <c r="AE9" s="8" t="n">
         <v>2070</v>
       </c>
-      <c r="AF9" s="5">
+      <c r="AF9" s="8" t="n">
         <v>2095</v>
       </c>
-      <c r="AG9" s="5">
+      <c r="AG9" s="8" t="n">
         <v>2120</v>
       </c>
-      <c r="AH9" s="5">
+      <c r="AH9" s="8" t="n">
         <v>2145</v>
       </c>
-      <c r="AI9" s="5">
+      <c r="AI9" s="8" t="n">
         <v>2170</v>
       </c>
-      <c r="AJ9" s="5">
+      <c r="AJ9" s="8" t="n">
         <v>2195</v>
       </c>
-      <c r="AK9" s="5">
+      <c r="AK9" s="8" t="n">
         <v>2220</v>
       </c>
-      <c r="AL9" s="5">
+      <c r="AL9" s="8" t="n">
         <v>2245</v>
       </c>
-      <c r="AM9" s="5">
+      <c r="AM9" s="8" t="n">
         <v>2270</v>
       </c>
-      <c r="AN9" s="5">
+      <c r="AN9" s="8" t="n">
         <v>2295</v>
       </c>
-      <c r="AO9" s="5">
+      <c r="AO9" s="8" t="n">
         <v>2320</v>
       </c>
-      <c r="AP9" s="5">
+      <c r="AP9" s="8" t="n">
         <v>2345</v>
       </c>
-      <c r="AQ9" s="5">
+      <c r="AQ9" s="8" t="n">
         <v>2370</v>
       </c>
-      <c r="AR9" s="5">
+      <c r="AR9" s="8" t="n">
         <v>2395</v>
       </c>
-      <c r="AS9" s="5">
+      <c r="AS9" s="8" t="n">
         <v>2420</v>
       </c>
-      <c r="AT9" s="5">
+      <c r="AT9" s="8" t="n">
         <v>2445</v>
       </c>
-      <c r="AU9" s="5">
+      <c r="AU9" s="8" t="n">
         <v>2470</v>
       </c>
-      <c r="AV9" s="5">
+      <c r="AV9" s="8" t="n">
         <v>2495</v>
       </c>
-      <c r="AW9" s="5">
+      <c r="AW9" s="8" t="n">
         <v>2520</v>
       </c>
-      <c r="AX9" s="5">
+      <c r="AX9" s="8" t="n">
         <v>2545</v>
       </c>
-      <c r="AY9" s="5">
+      <c r="AY9" s="8" t="n">
         <v>2570</v>
       </c>
-      <c r="AZ9" s="5">
+      <c r="AZ9" s="8" t="n">
         <v>2595</v>
       </c>
-      <c r="BA9" s="5">
+      <c r="BA9" s="8" t="n">
         <v>2620</v>
       </c>
-      <c r="BB9" s="5">
+      <c r="BB9" s="8" t="n">
         <v>2645</v>
       </c>
-      <c r="BC9" s="5">
+      <c r="BC9" s="8" t="n">
         <v>2670</v>
       </c>
-      <c r="BD9" s="5">
+      <c r="BD9" s="8" t="n">
         <v>2695</v>
       </c>
-      <c r="BE9" s="5">
+      <c r="BE9" s="8" t="n">
         <v>2720</v>
       </c>
-      <c r="BF9" s="5">
+      <c r="BF9" s="8" t="n">
         <v>2745</v>
       </c>
-      <c r="BG9" s="5">
+      <c r="BG9" s="8" t="n">
         <v>2770</v>
       </c>
-      <c r="BH9" s="5">
+      <c r="BH9" s="8" t="n">
         <v>2795</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7" t="n">
         <v>45054</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1" t="n">
         <v>15.6</v>
       </c>
-      <c r="AC10" s="9" t="s">
+      <c r="AC10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AD10" s="5">
+      <c r="AD10" s="8" t="n">
         <v>2040</v>
       </c>
-      <c r="AE10" s="5">
+      <c r="AE10" s="8" t="n">
         <v>2065</v>
       </c>
-      <c r="AF10" s="5">
+      <c r="AF10" s="8" t="n">
         <v>2090</v>
       </c>
-      <c r="AG10" s="5">
+      <c r="AG10" s="8" t="n">
         <v>2115</v>
       </c>
-      <c r="AH10" s="5">
+      <c r="AH10" s="8" t="n">
         <v>2140</v>
       </c>
-      <c r="AI10" s="5">
+      <c r="AI10" s="8" t="n">
         <v>2165</v>
       </c>
-      <c r="AJ10" s="5">
+      <c r="AJ10" s="8" t="n">
         <v>2190</v>
       </c>
-      <c r="AK10" s="5">
+      <c r="AK10" s="8" t="n">
         <v>2215</v>
       </c>
-      <c r="AL10" s="5">
+      <c r="AL10" s="8" t="n">
         <v>2240</v>
       </c>
-      <c r="AM10" s="5">
+      <c r="AM10" s="8" t="n">
         <v>2265</v>
       </c>
-      <c r="AN10" s="5">
+      <c r="AN10" s="8" t="n">
         <v>2290</v>
       </c>
-      <c r="AO10" s="5">
+      <c r="AO10" s="8" t="n">
         <v>2315</v>
       </c>
-      <c r="AP10" s="5">
+      <c r="AP10" s="8" t="n">
         <v>2340</v>
       </c>
-      <c r="AQ10" s="5">
+      <c r="AQ10" s="8" t="n">
         <v>2365</v>
       </c>
-      <c r="AR10" s="5">
+      <c r="AR10" s="8" t="n">
         <v>2390</v>
       </c>
-      <c r="AS10" s="5">
+      <c r="AS10" s="8" t="n">
         <v>2415</v>
       </c>
-      <c r="AT10" s="5">
+      <c r="AT10" s="8" t="n">
         <v>2440</v>
       </c>
-      <c r="AU10" s="5">
+      <c r="AU10" s="8" t="n">
         <v>2465</v>
       </c>
-      <c r="AV10" s="5">
+      <c r="AV10" s="8" t="n">
         <v>2490</v>
       </c>
-      <c r="AW10" s="5">
+      <c r="AW10" s="8" t="n">
         <v>2515</v>
       </c>
-      <c r="AX10" s="5">
+      <c r="AX10" s="8" t="n">
         <v>2540</v>
       </c>
-      <c r="AY10" s="5">
+      <c r="AY10" s="8" t="n">
         <v>2565</v>
       </c>
-      <c r="AZ10" s="5">
+      <c r="AZ10" s="8" t="n">
         <v>2590</v>
       </c>
-      <c r="BA10" s="5">
+      <c r="BA10" s="8" t="n">
         <v>2615</v>
       </c>
-      <c r="BB10" s="5">
+      <c r="BB10" s="8" t="n">
         <v>2640</v>
       </c>
-      <c r="BC10" s="5">
+      <c r="BC10" s="8" t="n">
         <v>2665</v>
       </c>
-      <c r="BD10" s="5">
+      <c r="BD10" s="8" t="n">
         <v>2690</v>
       </c>
-      <c r="BE10" s="5">
+      <c r="BE10" s="8" t="n">
         <v>2715</v>
       </c>
-      <c r="BF10" s="5">
+      <c r="BF10" s="8" t="n">
         <v>2740</v>
       </c>
-      <c r="BG10" s="5">
+      <c r="BG10" s="8" t="n">
         <v>2765</v>
       </c>
-      <c r="BH10" s="5">
+      <c r="BH10" s="8" t="n">
         <v>2790</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="7" t="n">
         <v>45055</v>
       </c>
-      <c r="D11">
-        <v>18.899999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="D11" s="1" t="n">
+        <v>18.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="7" t="n">
         <v>45056</v>
       </c>
-      <c r="D12">
-        <v>17.399999999999999</v>
+      <c r="D12" s="1" t="n">
+        <v>17.4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>